<commit_message>
fix empty warps line
</commit_message>
<xml_diff>
--- a/warps/checklist.xlsx
+++ b/warps/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/warps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB2D4F6-2022-DE42-8F06-D65CF0B6AC57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1CA5AC-8BB2-D24F-8FCF-214805652946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{8F973975-D728-DD43-939D-6FD780CCB81F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{8F973975-D728-DD43-939D-6FD780CCB81F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627EB446-E649-B74D-A499-EAD85EBC1807}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,9 +714,6 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>